<commit_message>
Some minor updates, nothing special
</commit_message>
<xml_diff>
--- a/character_names.xlsx
+++ b/character_names.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Human" sheetId="1" r:id="rId1"/>
+    <sheet name="Dwarf" sheetId="2" r:id="rId2"/>
+    <sheet name="Elf" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,10 +20,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,13 +70,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -331,12 +375,374 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>